<commit_message>
added MP Tower striplook
</commit_message>
<xml_diff>
--- a/EDDF/EDDF_strips.xlsx
+++ b/EDDF/EDDF_strips.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Games\Tower!Simulator3\ts3-basic-game-mods\EDDF\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC3B060-4D84-4F38-8D59-18FE52B7298D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Tower</t>
+  </si>
+  <si>
+    <t>ON FINAL</t>
+  </si>
+  <si>
+    <t>ARRIVAL 07L/25R</t>
+  </si>
+  <si>
+    <t>ARRIVAL 07C/25C</t>
+  </si>
+  <si>
+    <t>HANDOVER FROM GROUND</t>
+  </si>
+  <si>
+    <t>HANDOVER TO DEPARTURE</t>
+  </si>
+  <si>
+    <t>LINE UP 07L/25R</t>
+  </si>
+  <si>
+    <t>LINE UP 07C/25C</t>
+  </si>
+  <si>
+    <t>LINE UP 18</t>
+  </si>
+  <si>
+    <t>LINE UP 07R/25L</t>
+  </si>
+  <si>
+    <t>ARRIVAL 07R/25L</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +73,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,11 +105,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +388,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added EDDF MP Ground
</commit_message>
<xml_diff>
--- a/EDDF/EDDF_strips.xlsx
+++ b/EDDF/EDDF_strips.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Games\Tower!Simulator3\ts3-basic-game-mods\EDDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC3B060-4D84-4F38-8D59-18FE52B7298D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD15A067-B289-477D-9191-2477A65A7C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19305" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Tower</t>
   </si>
@@ -58,6 +58,33 @@
   </si>
   <si>
     <t>ARRIVAL 07R/25L</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>READY TO PUSHBACK</t>
+  </si>
+  <si>
+    <t>PUSHBACK</t>
+  </si>
+  <si>
+    <t>HANDOVER FROM TOWER</t>
+  </si>
+  <si>
+    <t>TAXI TO TERMINAL</t>
+  </si>
+  <si>
+    <t>TAXI 07L/25R</t>
+  </si>
+  <si>
+    <t>TAXI 07C/25C</t>
+  </si>
+  <si>
+    <t>TAXI 07R/25L</t>
+  </si>
+  <si>
+    <t>TAXI 18</t>
   </si>
 </sst>
 </file>
@@ -389,17 +416,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E4"/>
+  <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -442,6 +470,39 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>